<commit_message>
debug i2c; read data exec in mem function
</commit_message>
<xml_diff>
--- a/hardware/ravenna.xlsx
+++ b/hardware/ravenna.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10413"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jeffdi/Projects/ravenna/hardware/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B07472A-644B-5544-BD95-B07870AB061D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66CDCA40-48FA-2F43-A57D-FEB63038BF4C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-29580" yWindow="1720" windowWidth="27760" windowHeight="16940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3220" yWindow="2180" windowWidth="27760" windowHeight="16940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ravenna" sheetId="1" r:id="rId1"/>
@@ -965,7 +965,7 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -985,6 +985,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1341,15 +1343,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="A1:H25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection sqref="A1:F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="21"/>
   <cols>
-    <col min="1" max="1" width="21.625" customWidth="1"/>
+    <col min="1" max="1" width="52.75" style="10" customWidth="1"/>
     <col min="2" max="2" width="9.875" style="6" customWidth="1"/>
     <col min="3" max="3" width="20.25" style="4" customWidth="1"/>
     <col min="4" max="4" width="22.25" customWidth="1"/>
@@ -1360,7 +1365,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="2" customFormat="1">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="5" t="s">
@@ -1386,7 +1391,7 @@
       </c>
     </row>
     <row r="2" spans="1:8">
-      <c r="A2" t="s">
+      <c r="A2" s="10" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="6">
@@ -1412,7 +1417,7 @@
       </c>
     </row>
     <row r="3" spans="1:8">
-      <c r="A3" t="s">
+      <c r="A3" s="10" t="s">
         <v>7</v>
       </c>
       <c r="B3" s="6">
@@ -1438,7 +1443,7 @@
       </c>
     </row>
     <row r="4" spans="1:8">
-      <c r="A4" t="s">
+      <c r="A4" s="10" t="s">
         <v>9</v>
       </c>
       <c r="B4" s="6">
@@ -1464,7 +1469,7 @@
       </c>
     </row>
     <row r="5" spans="1:8">
-      <c r="A5" t="s">
+      <c r="A5" s="10" t="s">
         <v>12</v>
       </c>
       <c r="B5" s="6">
@@ -1484,7 +1489,7 @@
       </c>
     </row>
     <row r="6" spans="1:8">
-      <c r="A6" t="s">
+      <c r="A6" s="10" t="s">
         <v>15</v>
       </c>
       <c r="B6" s="6">
@@ -1510,7 +1515,7 @@
       </c>
     </row>
     <row r="7" spans="1:8">
-      <c r="A7" t="s">
+      <c r="A7" s="10" t="s">
         <v>18</v>
       </c>
       <c r="B7" s="6">
@@ -1536,7 +1541,7 @@
       </c>
     </row>
     <row r="8" spans="1:8">
-      <c r="A8" t="s">
+      <c r="A8" s="10" t="s">
         <v>21</v>
       </c>
       <c r="B8" s="6">
@@ -1562,7 +1567,7 @@
       </c>
     </row>
     <row r="9" spans="1:8">
-      <c r="A9" t="s">
+      <c r="A9" s="10" t="s">
         <v>24</v>
       </c>
       <c r="B9" s="6">
@@ -1588,7 +1593,7 @@
       </c>
     </row>
     <row r="10" spans="1:8">
-      <c r="A10" t="s">
+      <c r="A10" s="10" t="s">
         <v>26</v>
       </c>
       <c r="B10" s="6">
@@ -1614,7 +1619,7 @@
       </c>
     </row>
     <row r="11" spans="1:8">
-      <c r="A11" t="s">
+      <c r="A11" s="10" t="s">
         <v>29</v>
       </c>
       <c r="B11" s="6">
@@ -1640,7 +1645,7 @@
       </c>
     </row>
     <row r="12" spans="1:8">
-      <c r="A12" t="s">
+      <c r="A12" s="10" t="s">
         <v>32</v>
       </c>
       <c r="B12" s="6">
@@ -1666,7 +1671,7 @@
       </c>
     </row>
     <row r="13" spans="1:8">
-      <c r="A13" t="s">
+      <c r="A13" s="10" t="s">
         <v>35</v>
       </c>
       <c r="B13" s="6">
@@ -1692,7 +1697,7 @@
       </c>
     </row>
     <row r="14" spans="1:8">
-      <c r="A14" t="s">
+      <c r="A14" s="10" t="s">
         <v>38</v>
       </c>
       <c r="B14" s="6">
@@ -1718,7 +1723,7 @@
       </c>
     </row>
     <row r="15" spans="1:8">
-      <c r="A15" t="s">
+      <c r="A15" s="10" t="s">
         <v>41</v>
       </c>
       <c r="B15" s="6">
@@ -1744,7 +1749,7 @@
       </c>
     </row>
     <row r="16" spans="1:8">
-      <c r="A16" t="s">
+      <c r="A16" s="10" t="s">
         <v>42</v>
       </c>
       <c r="B16" s="6">
@@ -1770,7 +1775,7 @@
       </c>
     </row>
     <row r="17" spans="1:8">
-      <c r="A17" t="s">
+      <c r="A17" s="10" t="s">
         <v>43</v>
       </c>
       <c r="B17" s="6">
@@ -1796,7 +1801,7 @@
       </c>
     </row>
     <row r="18" spans="1:8">
-      <c r="A18" t="s">
+      <c r="A18" s="10" t="s">
         <v>45</v>
       </c>
       <c r="B18" s="6">
@@ -1822,7 +1827,7 @@
       </c>
     </row>
     <row r="19" spans="1:8">
-      <c r="A19" t="s">
+      <c r="A19" s="10" t="s">
         <v>47</v>
       </c>
       <c r="B19" s="6">
@@ -1848,7 +1853,7 @@
       </c>
     </row>
     <row r="20" spans="1:8">
-      <c r="A20" t="s">
+      <c r="A20" s="10" t="s">
         <v>50</v>
       </c>
       <c r="B20" s="6">
@@ -1874,7 +1879,7 @@
       </c>
     </row>
     <row r="21" spans="1:8">
-      <c r="A21" t="s">
+      <c r="A21" s="10" t="s">
         <v>52</v>
       </c>
       <c r="B21" s="6">
@@ -1900,7 +1905,7 @@
       </c>
     </row>
     <row r="22" spans="1:8">
-      <c r="A22" t="s">
+      <c r="A22" s="10" t="s">
         <v>56</v>
       </c>
       <c r="B22" s="6">
@@ -1926,7 +1931,7 @@
       </c>
     </row>
     <row r="23" spans="1:8">
-      <c r="A23" t="s">
+      <c r="A23" s="10" t="s">
         <v>59</v>
       </c>
       <c r="B23" s="6">
@@ -1952,7 +1957,7 @@
       </c>
     </row>
     <row r="24" spans="1:8">
-      <c r="A24" t="s">
+      <c r="A24" s="10" t="s">
         <v>64</v>
       </c>
       <c r="B24" s="6">
@@ -1978,7 +1983,7 @@
       </c>
     </row>
     <row r="25" spans="1:8">
-      <c r="A25" t="s">
+      <c r="A25" s="10" t="s">
         <v>64</v>
       </c>
       <c r="B25" s="6">
@@ -2030,5 +2035,6 @@
     <hyperlink ref="G10" r:id="rId23" xr:uid="{17CBC656-8371-9E44-A4D7-4D409583C8EE}"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup scale="33" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
update rtc; add nvram; update hardware;
</commit_message>
<xml_diff>
--- a/hardware/ravenna.xlsx
+++ b/hardware/ravenna.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jeffdi/Projects/ravenna/hardware/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66CDCA40-48FA-2F43-A57D-FEB63038BF4C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD94B69C-F1AC-744B-BD90-CF60D8FE0355}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3220" yWindow="2180" windowWidth="27760" windowHeight="16940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5640" yWindow="1620" windowWidth="27760" windowHeight="16940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ravenna" sheetId="1" r:id="rId1"/>
@@ -1349,7 +1349,7 @@
   <dimension ref="A1:H25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection sqref="A1:F25"/>
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="21"/>
@@ -1961,7 +1961,7 @@
         <v>64</v>
       </c>
       <c r="B24" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C24" s="4" t="s">
         <v>65</v>

</xml_diff>